<commit_message>
completed bill view page
</commit_message>
<xml_diff>
--- a/customTemplate/mandaysClaimed/customTemplateMandays.xlsx
+++ b/customTemplate/mandaysClaimed/customTemplateMandays.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab0ca60d3e11cd5c/Desktop/mandaysClaimed/customTemplate/mandaysClaimed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab0ca60d3e11cd5c/Desktop/hrManagementSystem/customTemplate/mandaysClaimed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{CAB2FB5C-17ED-4DA2-98F5-A6A6CE9C41CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09BEA8E9-83C5-475E-95AB-5E4F8DE89112}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{CAB2FB5C-17ED-4DA2-98F5-A6A6CE9C41CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33EF6059-C88D-48A8-9B46-5AF0A75BC3CC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{67CF385C-F394-4104-8FDA-3471314286F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WD</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>DSM</t>
+  </si>
+  <si>
+    <t>Designation</t>
   </si>
 </sst>
 </file>
@@ -113,10 +116,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,7 +418,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,6 +433,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -470,5 +472,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>